<commit_message>
threaded tkinter made to work
changed the logic to update position for each pixel from threads.
</commit_message>
<xml_diff>
--- a/miniWarehouseData.xlsx
+++ b/miniWarehouseData.xlsx
@@ -284,7 +284,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B10"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -336,7 +336,6 @@
         <v>8</v>
       </c>
       <c r="G2" s="4" t="n">
-        <f aca="false">RANDBETWEEN(0,4)</f>
         <v>0</v>
       </c>
     </row>
@@ -358,7 +357,7 @@
       </c>
       <c r="F3" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G3" s="4" t="n">
         <f aca="false">RANDBETWEEN(0,4)</f>
@@ -387,7 +386,7 @@
       </c>
       <c r="G4" s="4" t="n">
         <f aca="false">RANDBETWEEN(0,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -412,7 +411,7 @@
       </c>
       <c r="G5" s="4" t="n">
         <f aca="false">RANDBETWEEN(0,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,7 +436,7 @@
       </c>
       <c r="G6" s="4" t="n">
         <f aca="false">RANDBETWEEN(0,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -462,7 +461,7 @@
       </c>
       <c r="G7" s="4" t="n">
         <f aca="false">RANDBETWEEN(0,4)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,7 +486,7 @@
       </c>
       <c r="G8" s="4" t="n">
         <f aca="false">RANDBETWEEN(0,4)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,7 +511,7 @@
       </c>
       <c r="G9" s="4" t="n">
         <f aca="false">RANDBETWEEN(0,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,7 +536,7 @@
       </c>
       <c r="G10" s="4" t="n">
         <f aca="false">RANDBETWEEN(0,4)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>